<commit_message>
add function to export ocr output to eagle eye excel formate
</commit_message>
<xml_diff>
--- a/media/financial_output/cimb/output_cimb_statement1.xlsx
+++ b/media/financial_output/cimb/output_cimb_statement1.xlsx
@@ -481,27 +481,27 @@
     <t>date</t>
   </si>
   <si>
-    <t>T6-1806128-3
+    <t>T6-18060128-3
 _x000C_</t>
   </si>
   <si>
-    <t>NUR IZZAHTI BINTI AZEMAN
+    <t>NUR IZZAHTI BINT! AZEMAN
 _x000C_</t>
   </si>
   <si>
     <t>NO 19 JALAN Nd FASA DA
 TAMAN MELAWATI
 KUALA LUMPUR
-53100 SELANGOR SELANGOR
+53100 SELANGOR, SELANGOR
 _x000C_</t>
   </si>
   <si>
-    <t>150H2020
+    <t>10R2020
 _x000C_</t>
   </si>
   <si>
     <t>UR IZZAHTI BINT! AZEM
-3419 JALAN Ald FASA OA
+7419 JALAN Ald FASA GA
 _x000C_</t>
   </si>
 </sst>

</xml_diff>